<commit_message>
Se añade escenario Descarga de Poliza
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/DataReembolso.xlsx
+++ b/src/test/resources/dataDriven/DataReembolso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candyespinzabaez/Documents/Proyecto APP/CanalApp-auto-Android-test-v1/src/test/resources/dataDriven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC31C58-E5A4-AA40-8A6C-7CADDB7B51CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F955A-60FC-F744-83E3-2084D6B31D49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="2280" windowWidth="30560" windowHeight="10540" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
+    <workbookView xWindow="18500" yWindow="6240" windowWidth="30560" windowHeight="10540" xr2:uid="{897FEA26-AEC5-9349-951A-1C74BA5F166B}"/>
   </bookViews>
   <sheets>
     <sheet name="01-SegReembolso" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>usar</t>
   </si>
@@ -53,9 +53,6 @@
     <t>montoReembolso</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -68,22 +65,7 @@
     <t>Rimac2020</t>
   </si>
   <si>
-    <t>723</t>
-  </si>
-  <si>
-    <t>76243722</t>
-  </si>
-  <si>
-    <t>Rimac2021</t>
-  </si>
-  <si>
-    <t>348</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>150</t>
+    <t>209</t>
   </si>
 </sst>
 </file>
@@ -444,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B50BC4-0409-6D4F-9E89-E81C3373F2D1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="A2:E6"/>
+      <selection activeCell="A3" sqref="A3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,72 +458,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>